<commit_message>
Complete First Steps with Sass Mixins Extends and Functions
</commit_message>
<xml_diff>
--- a/SASS/Notebook.xlsx
+++ b/SASS/Notebook.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21601"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F8693C5-CCC7-43A2-9C29-0EEB9D4A957F}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A46CFE7B-383B-4D85-B0F8-12A4147223D5}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,12 +20,18 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>Day 1 (27/05/2019)</t>
   </si>
   <si>
     <t>Complete First Steps with Sass Variables and Nesting</t>
+  </si>
+  <si>
+    <t>Day 2 (28/05/2019)</t>
+  </si>
+  <si>
+    <t>Complete First Steps with Sass Mixins Extends and Functions</t>
   </si>
 </sst>
 </file>
@@ -343,16 +349,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B1"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="29.140625" customWidth="1"/>
-    <col min="2" max="2" width="55" customWidth="1"/>
+    <col min="2" max="2" width="57" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -363,6 +369,14 @@
         <v>1</v>
       </c>
     </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
update day 3 learning SCSS
</commit_message>
<xml_diff>
--- a/SASS/Notebook.xlsx
+++ b/SASS/Notebook.xlsx
@@ -3,35 +3,57 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21601"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A46CFE7B-383B-4D85-B0F8-12A4147223D5}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7166A97-8258-4CD8-82DC-F2A0BCC5CA81}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="345" yWindow="1020" windowWidth="15375" windowHeight="7875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
-  <si>
-    <t>Day 1 (27/05/2019)</t>
-  </si>
-  <si>
-    <t>Complete First Steps with Sass Variables and Nesting</t>
-  </si>
-  <si>
-    <t>Day 2 (28/05/2019)</t>
-  </si>
-  <si>
-    <t>Complete First Steps with Sass Mixins Extends and Functions</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+  <si>
+    <t>Day 1 (26/05/2019)</t>
+  </si>
+  <si>
+    <t>Day 2 (27/05/2019)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Learning how to install scss with node
+Learning one CSS property =&gt; clip-path 
+</t>
+  </si>
+  <si>
+    <t>Day 3 (28/05/2019)</t>
+  </si>
+  <si>
+    <t>Day 4 (29/05/2019)</t>
+  </si>
+  <si>
+    <t>Day 5 (30/05/2019)</t>
+  </si>
+  <si>
+    <t>Day 6 (31/05/2019)</t>
+  </si>
+  <si>
+    <t>Learning using Sass Mixins Extends and Functions</t>
+  </si>
+  <si>
+    <t>Learning using Sass Variables and Nesting</t>
   </si>
 </sst>
 </file>
@@ -67,8 +89,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -349,35 +380,59 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="29.140625" customWidth="1"/>
-    <col min="2" max="2" width="57" customWidth="1"/>
+    <col min="1" max="1" width="25.42578125" customWidth="1"/>
+    <col min="2" max="2" width="71.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="B2" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B2" t="s">
-        <v>3</v>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>6</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Converting Our CSS Code to Sass Variables and Nesting
</commit_message>
<xml_diff>
--- a/SASS/Notebook.xlsx
+++ b/SASS/Notebook.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21629"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7166A97-8258-4CD8-82DC-F2A0BCC5CA81}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3E59773-1EF4-4C2F-8A09-09FED4C68732}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="345" yWindow="1020" windowWidth="15375" windowHeight="7875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="150" yWindow="1665" windowWidth="15375" windowHeight="7875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>Day 1 (26/05/2019)</t>
   </si>
@@ -41,9 +41,6 @@
     <t>Day 3 (28/05/2019)</t>
   </si>
   <si>
-    <t>Day 4 (29/05/2019)</t>
-  </si>
-  <si>
     <t>Day 5 (30/05/2019)</t>
   </si>
   <si>
@@ -54,6 +51,12 @@
   </si>
   <si>
     <t>Learning using Sass Variables and Nesting</t>
+  </si>
+  <si>
+    <t>Day 4 (26/06/2019)</t>
+  </si>
+  <si>
+    <t>Learning Converting Our CSS Code to Sass Variables and Nesting =&gt; Implement to the Natours Project</t>
   </si>
 </sst>
 </file>
@@ -383,13 +386,13 @@
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="25.42578125" customWidth="1"/>
-    <col min="2" max="2" width="71.85546875" customWidth="1"/>
+    <col min="2" max="2" width="89.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -397,7 +400,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -405,7 +408,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="45" x14ac:dyDescent="0.25">
@@ -418,17 +421,20 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>4</v>
+        <v>8</v>
+      </c>
+      <c r="B4" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
SASS Learning/Complete buidling about section for project number 1
</commit_message>
<xml_diff>
--- a/SASS/Notebook.xlsx
+++ b/SASS/Notebook.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21629"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA400ACE-0608-4116-B1E1-9198AA574E84}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BBA81BF-DF67-4673-B13F-14D2C1F3B69F}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4980" yWindow="3045" windowWidth="15375" windowHeight="7875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>Day 1 (26/05/2019)</t>
   </si>
@@ -41,9 +41,6 @@
     <t>Day 3 (28/05/2019)</t>
   </si>
   <si>
-    <t>Day 6 (31/05/2019)</t>
-  </si>
-  <si>
     <t>Learning using Sass Mixins Extends and Functions</t>
   </si>
   <si>
@@ -59,7 +56,19 @@
     <t>Day 5 (27/06/2019)</t>
   </si>
   <si>
-    <t xml:space="preserve"> Learning how to implementing the 7-1 CSS Architecture with Sass, how to organizing scss file structure</t>
+    <t>Day 6 (29/06/2019)</t>
+  </si>
+  <si>
+    <t>Learning how to implementing the 7-1 CSS Architecture with Sass, how to organizing scss file structure</t>
+  </si>
+  <si>
+    <t>Learning how to building a custom grid with floats, using :not() pseudo</t>
+  </si>
+  <si>
+    <t>Day 7 (30/06/2019)</t>
+  </si>
+  <si>
+    <t>Completing how to building about section with SASS_Natours Project</t>
   </si>
 </sst>
 </file>
@@ -386,7 +395,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B10" sqref="B10"/>
@@ -395,7 +404,7 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="25.42578125" customWidth="1"/>
-    <col min="2" max="2" width="89.28515625" customWidth="1"/>
+    <col min="2" max="2" width="101.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -403,7 +412,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -411,7 +420,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="45" x14ac:dyDescent="0.25">
@@ -424,15 +433,15 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" t="s">
         <v>7</v>
-      </c>
-      <c r="B4" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B5" t="s">
         <v>10</v>
@@ -440,7 +449,18 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>4</v>
+        <v>9</v>
+      </c>
+      <c r="B6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
SASS Learning/Complete buidling the Tours Section for project number 1
</commit_message>
<xml_diff>
--- a/SASS/Notebook.xlsx
+++ b/SASS/Notebook.xlsx
@@ -1,16 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21727"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BBA81BF-DF67-4673-B13F-14D2C1F3B69F}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{0BEEC7BC-EC8A-46C3-815C-3476DDC3A248}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4980" yWindow="3045" windowWidth="15375" windowHeight="7875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="181029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>Day 1 (26/05/2019)</t>
   </si>
@@ -69,6 +70,18 @@
   </si>
   <si>
     <t>Completing how to building about section with SASS_Natours Project</t>
+  </si>
+  <si>
+    <t>Day 8, 9 (4-5/07/2019</t>
+  </si>
+  <si>
+    <t>Learn about new CSS brand feature: background-blend-mode, box-decoration-break</t>
+  </si>
+  <si>
+    <t>Day 10 (6/07/2019</t>
+  </si>
+  <si>
+    <t>Learn how to use over-flow: hidden when before we used clip-path</t>
   </si>
 </sst>
 </file>
@@ -395,10 +408,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -463,6 +476,22 @@
         <v>13</v>
       </c>
     </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9" t="s">
+        <v>17</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Building the Stories Section - Part 1 --- Natour Project
</commit_message>
<xml_diff>
--- a/SASS/Notebook.xlsx
+++ b/SASS/Notebook.xlsx
@@ -1,17 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21727"/>
-  <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0BEEC7BC-EC8A-46C3-815C-3476DDC3A248}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
-  <fileRecoveryPr repairLoad="1"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -26,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>Day 1 (26/05/2019)</t>
   </si>
@@ -72,24 +70,61 @@
     <t>Completing how to building about section with SASS_Natours Project</t>
   </si>
   <si>
-    <t>Day 8, 9 (4-5/07/2019</t>
-  </si>
-  <si>
     <t>Learn about new CSS brand feature: background-blend-mode, box-decoration-break</t>
   </si>
   <si>
-    <t>Day 10 (6/07/2019</t>
-  </si>
-  <si>
     <t>Learn how to use over-flow: hidden when before we used clip-path</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Learing new some properties: </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">shape-outside: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>define where the content floats around the element =&gt; if you actually want the element to look lije that circle, we can then use the clip-path property</t>
+    </r>
+  </si>
+  <si>
+    <t>Day 8, 9 (04-05/07/2019</t>
+  </si>
+  <si>
+    <t>Day 10 (06/07/2019</t>
+  </si>
+  <si>
+    <t>Day 11 (08/07/2019</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -407,11 +442,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B9"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -478,18 +513,26 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B8" t="s">
         <v>14</v>
-      </c>
-      <c r="B8" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B9" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B10" t="s">
         <v>16</v>
-      </c>
-      <c r="B9" t="s">
-        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>